<commit_message>
updates .xls for EST-1571 analysis
</commit_message>
<xml_diff>
--- a/adocs/documentation/src/main/asciidoc/discussion-papers/linking-immutable-invoices.xlsx
+++ b/adocs/documentation/src/main/asciidoc/discussion-papers/linking-immutable-invoices.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37470" windowHeight="18195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37470" windowHeight="18195" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="link immutable, same supplier" sheetId="1" r:id="rId1"/>
     <sheet name="link immutable, diff supplier" sheetId="2" r:id="rId2"/>
+    <sheet name="link immutable, multi order itm" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="60">
   <si>
     <t>Invoice</t>
   </si>
@@ -144,9 +145,6 @@
     <t>link?</t>
   </si>
   <si>
-    <t>---</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -193,6 +191,21 @@
   </si>
   <si>
     <t>AND link to order:</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>WHEN realised should be linked to multiiple order items with different charges, but for the same supplier, eg:</t>
+  </si>
+  <si>
+    <t>AND split the new item</t>
+  </si>
+  <si>
+    <t>split out, 700 to charge code 'Z'</t>
+  </si>
+  <si>
+    <t>-linked-</t>
   </si>
 </sst>
 </file>
@@ -553,9 +566,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +622,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -639,7 +652,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -663,7 +676,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -705,7 +718,7 @@
         <v>36</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -722,12 +735,12 @@
         <v>37</v>
       </c>
       <c r="N15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -786,7 +799,7 @@
         <v>2000</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="J21" t="s">
         <v>9</v>
@@ -801,7 +814,7 @@
         <v>37</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -907,7 +920,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +974,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -991,20 +1004,20 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -1015,7 +1028,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1057,7 +1070,7 @@
         <v>36</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1074,12 +1087,12 @@
         <v>37</v>
       </c>
       <c r="N15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1123,7 +1136,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" t="s">
         <v>22</v>
@@ -1132,7 +1145,7 @@
         <v>37</v>
       </c>
       <c r="N21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1151,21 +1164,21 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M25" t="s">
         <v>37</v>
       </c>
       <c r="N25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -1184,26 +1197,26 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" t="s">
         <v>40</v>
       </c>
-      <c r="H30" t="s">
-        <v>41</v>
-      </c>
       <c r="I30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" t="s">
         <v>24</v>
@@ -1212,7 +1225,7 @@
         <v>2000</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="J31" t="s">
         <v>7</v>
@@ -1322,6 +1335,490 @@
         <v>19</v>
       </c>
       <c r="D68" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5">
+        <v>1000</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9">
+        <v>2000</v>
+      </c>
+      <c r="G9" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11">
+        <v>5000</v>
+      </c>
+      <c r="G11" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15">
+        <v>1000</v>
+      </c>
+      <c r="M15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="1">
+        <v>-1000</v>
+      </c>
+      <c r="M16" t="s">
+        <v>36</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17">
+        <v>1000</v>
+      </c>
+      <c r="M17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21">
+        <v>1000</v>
+      </c>
+      <c r="M21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" s="1">
+        <v>-1000</v>
+      </c>
+      <c r="M22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23">
+        <v>300</v>
+      </c>
+      <c r="M23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" t="s">
+        <v>55</v>
+      </c>
+      <c r="L24">
+        <v>700</v>
+      </c>
+      <c r="M24" t="s">
+        <v>37</v>
+      </c>
+      <c r="N24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" t="s">
+        <v>24</v>
+      </c>
+      <c r="L28">
+        <v>1000</v>
+      </c>
+      <c r="M28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="1">
+        <v>-1000</v>
+      </c>
+      <c r="M29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30">
+        <v>2000</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J30" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" t="s">
+        <v>24</v>
+      </c>
+      <c r="L30">
+        <v>300</v>
+      </c>
+      <c r="M30" t="s">
+        <v>37</v>
+      </c>
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32">
+        <v>5000</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" t="s">
+        <v>55</v>
+      </c>
+      <c r="L32">
+        <v>700</v>
+      </c>
+      <c r="M32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>2</v>
+      </c>
+      <c r="I55" t="s">
+        <v>3</v>
+      </c>
+      <c r="L55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>7</v>
+      </c>
+      <c r="I56" t="s">
+        <v>8</v>
+      </c>
+      <c r="L56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57">
+        <v>600</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>11</v>
+      </c>
+      <c r="I58" t="s">
+        <v>12</v>
+      </c>
+      <c r="L58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" t="s">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>